<commit_message>
Add more 2ndphase reducers
</commit_message>
<xml_diff>
--- a/boundary/results2.xlsx
+++ b/boundary/results2.xlsx
@@ -868,6 +868,7 @@
   <fonts count="8">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -889,24 +890,26 @@
     <font>
       <name val="Arial"/>
       <family val="2"/>
+      <b val="true"/>
       <color rgb="003C3C3C"/>
       <sz val="13"/>
     </font>
     <font>
       <name val="Arial"/>
       <family val="2"/>
-      <color rgb="003C3C3C"/>
       <sz val="10"/>
     </font>
     <font>
       <name val="Arial"/>
       <family val="2"/>
+      <b val="true"/>
       <color rgb="003C3C3C"/>
       <sz val="9"/>
     </font>
     <font>
       <name val="Arial"/>
       <family val="2"/>
+      <b val="true"/>
       <sz val="13"/>
     </font>
   </fonts>
@@ -1052,7 +1055,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1067,7 +1070,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300">
+              <a:rPr b="1" sz="1300">
                 <a:solidFill>
                   <a:srgbClr val="3c3c3c"/>
                 </a:solidFill>
@@ -1322,11 +1325,11 @@
         </c:ser>
         <c:overlap val="100"/>
         <c:gapWidth val="100"/>
-        <c:axId val="26069215"/>
-        <c:axId val="93146828"/>
+        <c:axId val="41347432"/>
+        <c:axId val="65789398"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="26069215"/>
+        <c:axId val="41347432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1341,7 +1344,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900">
+                  <a:rPr b="1" sz="900">
                     <a:solidFill>
                       <a:srgbClr val="3c3c3c"/>
                     </a:solidFill>
@@ -1356,7 +1359,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93146828"/>
+        <c:crossAx val="65789398"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
@@ -1370,7 +1373,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93146828"/>
+        <c:axId val="65789398"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1385,7 +1388,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900">
+                  <a:rPr b="1" sz="900">
                     <a:solidFill>
                       <a:srgbClr val="3c3c3c"/>
                     </a:solidFill>
@@ -1409,7 +1412,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="26069215"/>
+        <c:crossAx val="41347432"/>
         <c:crossesAt val="1"/>
         <c:spPr>
           <a:ln>
@@ -1441,7 +1444,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1456,7 +1459,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300">
+              <a:rPr b="1" sz="1300">
                 <a:solidFill>
                   <a:srgbClr val="3c3c3c"/>
                 </a:solidFill>
@@ -1750,11 +1753,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="59284914"/>
-        <c:axId val="4401127"/>
+        <c:axId val="37193386"/>
+        <c:axId val="9291117"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="59284914"/>
+        <c:axId val="37193386"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="210"/>
@@ -1763,7 +1766,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="4401127"/>
+        <c:crossAx val="9291117"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
@@ -1774,7 +1777,7 @@
         </c:spPr>
       </c:valAx>
       <c:valAx>
-        <c:axId val="4401127"/>
+        <c:axId val="9291117"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1791,7 +1794,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59284914"/>
+        <c:crossAx val="37193386"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
@@ -1823,7 +1826,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2164,11 +2167,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="83190370"/>
-        <c:axId val="31367459"/>
+        <c:axId val="87399537"/>
+        <c:axId val="76106620"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="83190370"/>
+        <c:axId val="87399537"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2176,7 +2179,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="31367459"/>
+        <c:crossAx val="76106620"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
@@ -2187,7 +2190,7 @@
         </c:spPr>
       </c:valAx>
       <c:valAx>
-        <c:axId val="31367459"/>
+        <c:axId val="76106620"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2204,7 +2207,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83190370"/>
+        <c:crossAx val="87399537"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
@@ -2236,7 +2239,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2251,7 +2254,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300">
+              <a:rPr b="1" sz="1300">
                 <a:solidFill>
                   <a:srgbClr val="3c3c3c"/>
                 </a:solidFill>
@@ -2527,11 +2530,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="47700698"/>
-        <c:axId val="41461683"/>
+        <c:axId val="8586539"/>
+        <c:axId val="43061618"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="47700698"/>
+        <c:axId val="8586539"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2539,7 +2542,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41461683"/>
+        <c:crossAx val="43061618"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
@@ -2550,7 +2553,7 @@
         </c:spPr>
       </c:valAx>
       <c:valAx>
-        <c:axId val="41461683"/>
+        <c:axId val="43061618"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2567,7 +2570,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47700698"/>
+        <c:crossAx val="8586539"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
@@ -2599,7 +2602,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2614,7 +2617,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300"/>
+              <a:rPr b="1" sz="1300"/>
               <a:t>No object equalization</a:t>
             </a:r>
           </a:p>
@@ -2687,25 +2690,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>80</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>80</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>80</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>81</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>82</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>82</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>84</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2773,25 +2776,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>240</c:v>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>282</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>318</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>342</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>362</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>368</c:v>
+                  <c:v>101</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>379</c:v>
+                  <c:v>102</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2859,35 +2862,35 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>54</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>56</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>56</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>58</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>60</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="80290942"/>
-        <c:axId val="88363106"/>
+        <c:axId val="48395512"/>
+        <c:axId val="73677920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80290942"/>
+        <c:axId val="48395512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2895,8 +2898,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88363106"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="73677920"/>
+        <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
             <a:solidFill>
@@ -2906,7 +2909,7 @@
         </c:spPr>
       </c:valAx>
       <c:valAx>
-        <c:axId val="88363106"/>
+        <c:axId val="73677920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2923,8 +2926,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80290942"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="48395512"/>
+        <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
             <a:solidFill>
@@ -2955,7 +2958,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2970,7 +2973,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300"/>
+              <a:rPr b="1" sz="1300"/>
               <a:t>With object # equalization</a:t>
             </a:r>
           </a:p>
@@ -3007,35 +3010,6 @@
             </a:ln>
           </c:spPr>
           <c:marker/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$101:$H$101</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.00%</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.29%</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.56%</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.78%</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.99%</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.16%</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.30%</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:yVal>
             <c:numRef>
               <c:f>Sheet1!$B$102:$H$102</c:f>
@@ -3093,35 +3067,6 @@
             </a:ln>
           </c:spPr>
           <c:marker/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$101:$H$101</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.00%</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.29%</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.56%</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.78%</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.99%</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.16%</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.30%</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:yVal>
             <c:numRef>
               <c:f>Sheet1!$B$103:$H$103</c:f>
@@ -3129,25 +3074,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>258.96</c:v>
+                  <c:v>98.189</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>300.33</c:v>
+                  <c:v>97.98</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>334.218</c:v>
+                  <c:v>96.692</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>354.996</c:v>
+                  <c:v>100.686</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>371.05</c:v>
+                  <c:v>102.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>372.5264</c:v>
+                  <c:v>102.2423</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>379</c:v>
+                  <c:v>102</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3179,35 +3124,6 @@
             </a:ln>
           </c:spPr>
           <c:marker/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$101:$H$101</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.00%</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.29%</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.56%</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.78%</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.99%</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.16%</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.30%</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:yVal>
             <c:numRef>
               <c:f>Sheet1!$B$104:$H$104</c:f>
@@ -3239,11 +3155,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="51687163"/>
-        <c:axId val="19902499"/>
+        <c:axId val="73632381"/>
+        <c:axId val="68146225"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="51687163"/>
+        <c:axId val="73632381"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3251,8 +3167,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="19902499"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="68146225"/>
+        <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
             <a:solidFill>
@@ -3262,7 +3178,7 @@
         </c:spPr>
       </c:valAx>
       <c:valAx>
-        <c:axId val="19902499"/>
+        <c:axId val="68146225"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3279,8 +3195,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51687163"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="73632381"/>
+        <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
             <a:solidFill>
@@ -3315,16 +3231,16 @@
 <xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>801720</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>11880</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>93960</xdr:rowOff>
+      <xdr:rowOff>84960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>478800</xdr:colOff>
+      <xdr:colOff>505440</xdr:colOff>
       <xdr:row>75</xdr:row>
-      <xdr:rowOff>67680</xdr:rowOff>
+      <xdr:rowOff>58320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3332,8 +3248,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="16250400" y="8868960"/>
-        <a:ext cx="8911800" cy="4632120"/>
+        <a:off x="16352280" y="8727840"/>
+        <a:ext cx="8954640" cy="4565520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3346,15 +3262,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>128520</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>2880</xdr:rowOff>
+      <xdr:colOff>155520</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>172800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>707400</xdr:colOff>
+      <xdr:colOff>734040</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>16200</xdr:rowOff>
+      <xdr:rowOff>6840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3362,8 +3278,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="128520" y="181800"/>
-        <a:ext cx="5762880" cy="3237120"/>
+        <a:off x="155520" y="172800"/>
+        <a:ext cx="5787720" cy="3236760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3376,15 +3292,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>76320</xdr:colOff>
+      <xdr:colOff>103320</xdr:colOff>
       <xdr:row>65</xdr:row>
-      <xdr:rowOff>29880</xdr:rowOff>
+      <xdr:rowOff>20880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>263520</xdr:colOff>
+      <xdr:colOff>290160</xdr:colOff>
       <xdr:row>89</xdr:row>
-      <xdr:rowOff>149040</xdr:rowOff>
+      <xdr:rowOff>139680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3392,8 +3308,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8698320" y="11671920"/>
-        <a:ext cx="7013880" cy="4418640"/>
+        <a:off x="8767080" y="11481120"/>
+        <a:ext cx="7046640" cy="4352400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3406,15 +3322,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>671040</xdr:colOff>
+      <xdr:colOff>698040</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>158400</xdr:colOff>
+      <xdr:colOff>185040</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>150120</xdr:rowOff>
+      <xdr:rowOff>149760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3422,8 +3338,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7667280" y="0"/>
-        <a:ext cx="7499160" cy="4806360"/>
+        <a:off x="7728480" y="0"/>
+        <a:ext cx="7536960" cy="4806000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3436,15 +3352,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>294480</xdr:colOff>
+      <xdr:colOff>321480</xdr:colOff>
       <xdr:row>82</xdr:row>
-      <xdr:rowOff>168120</xdr:rowOff>
+      <xdr:rowOff>159120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>480960</xdr:colOff>
+      <xdr:colOff>507600</xdr:colOff>
       <xdr:row>101</xdr:row>
-      <xdr:rowOff>3960</xdr:rowOff>
+      <xdr:rowOff>3600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3452,8 +3368,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8103600" y="14855400"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="8168760" y="14631840"/>
+        <a:ext cx="5785920" cy="3173040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3465,16 +3381,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>56520</xdr:colOff>
-      <xdr:row>81</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>672840</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>174600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>195120</xdr:colOff>
-      <xdr:row>99</xdr:row>
-      <xdr:rowOff>178920</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>74520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3482,8 +3398,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1428480" y="14677560"/>
-        <a:ext cx="5762880" cy="3234240"/>
+        <a:off x="7703280" y="18676440"/>
+        <a:ext cx="5789520" cy="3167640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3504,36 +3420,36 @@
   <dimension ref="A1:X106"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A81" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="H104" activeCellId="0" pane="topLeft" sqref="H104"/>
+      <selection activeCell="H97" activeCellId="0" pane="topLeft" sqref="H97"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5450980392157"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5764705882353"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.65490196078431"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="17.0313725490196"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.5764705882353"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.2352941176471"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="11.5764705882353"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.0235294117647"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.5764705882353"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.25490196078431"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.6078431372549"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="11.5764705882353"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="4.18823529411765"/>
-    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="11.5764705882353"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="6.27843137254902"/>
-    <col collapsed="false" hidden="false" max="21" min="20" style="0" width="11.5764705882353"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="4.18823529411765"/>
-    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.643137254902"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.70196078431373"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="17.1137254901961"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.3098039215686"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.078431372549"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.29019607843137"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.6627450980392"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="4.20392156862745"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="6.31372549019608"/>
+    <col collapsed="false" hidden="false" max="21" min="20" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="4.20392156862745"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="1">
       <c r="F1" s="0" t="n">
         <v>1024</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
         <v>0</v>
       </c>
@@ -3565,7 +3481,7 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="3">
       <c r="E3" s="0" t="s">
         <v>3</v>
       </c>
@@ -3609,7 +3525,7 @@
         <v>0.189496</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="4">
       <c r="E4" s="0" t="s">
         <v>10</v>
       </c>
@@ -3653,7 +3569,7 @@
         <v>0.201653</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="5">
       <c r="E5" s="0" t="s">
         <v>17</v>
       </c>
@@ -3697,7 +3613,7 @@
         <v>0.182607</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="6">
       <c r="E6" s="0" t="s">
         <v>24</v>
       </c>
@@ -3741,7 +3657,7 @@
         <v>0.19657</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="7">
       <c r="E7" s="0" t="s">
         <v>31</v>
       </c>
@@ -3785,7 +3701,7 @@
         <v>0.198864</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="8">
       <c r="E8" s="0" t="s">
         <v>38</v>
       </c>
@@ -3829,7 +3745,7 @@
         <v>0.221156</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="9">
       <c r="E9" s="0" t="s">
         <v>45</v>
       </c>
@@ -3873,7 +3789,7 @@
         <v>0.216609</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="10">
       <c r="E10" s="0" t="s">
         <v>52</v>
       </c>
@@ -3917,7 +3833,7 @@
         <v>0.232622</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="11">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="11">
       <c r="E11" s="0" t="s">
         <v>59</v>
       </c>
@@ -3961,7 +3877,7 @@
         <v>0.17561</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="12">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="12">
       <c r="E12" s="0" t="s">
         <v>66</v>
       </c>
@@ -4005,7 +3921,7 @@
         <v>0.19074</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="13">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="13">
       <c r="E13" s="0" t="s">
         <v>73</v>
       </c>
@@ -4049,7 +3965,7 @@
         <v>0.208292</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="14">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="14">
       <c r="E14" s="0" t="s">
         <v>80</v>
       </c>
@@ -4093,7 +4009,7 @@
         <v>0.226985</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="15">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="15">
       <c r="E15" s="0" t="s">
         <v>87</v>
       </c>
@@ -4137,7 +4053,7 @@
         <v>0.181498</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="16">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="16">
       <c r="E16" s="0" t="s">
         <v>94</v>
       </c>
@@ -4181,7 +4097,7 @@
         <v>0.194111</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="17">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="17">
       <c r="E17" s="0" t="s">
         <v>101</v>
       </c>
@@ -4225,7 +4141,7 @@
         <v>0.195362</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="18">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="18">
       <c r="E18" s="0" t="s">
         <v>108</v>
       </c>
@@ -4269,7 +4185,7 @@
         <v>0.212927</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="19">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="19">
       <c r="E19" s="0" t="s">
         <v>115</v>
       </c>
@@ -4313,7 +4229,7 @@
         <v>0.166839</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="20">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="20">
       <c r="E20" s="0" t="s">
         <v>122</v>
       </c>
@@ -4357,7 +4273,7 @@
         <v>0.184421</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="21">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="21">
       <c r="E21" s="0" t="s">
         <v>129</v>
       </c>
@@ -4401,7 +4317,7 @@
         <v>0.171104</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="22">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="22">
       <c r="E22" s="0" t="s">
         <v>136</v>
       </c>
@@ -4445,7 +4361,7 @@
         <v>0.18754</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="23">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="23">
       <c r="E23" s="0" t="s">
         <v>143</v>
       </c>
@@ -4489,7 +4405,7 @@
         <v>0.20713</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="24">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="24">
       <c r="E24" s="0" t="s">
         <v>150</v>
       </c>
@@ -4533,7 +4449,7 @@
         <v>0.219554</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="25">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="25">
       <c r="E25" s="0" t="s">
         <v>157</v>
       </c>
@@ -4577,7 +4493,7 @@
         <v>0.184317</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="26">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="26">
       <c r="E26" s="0" t="s">
         <v>164</v>
       </c>
@@ -4621,7 +4537,7 @@
         <v>0.197411</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="27">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="27">
       <c r="E27" s="0" t="s">
         <v>171</v>
       </c>
@@ -4665,7 +4581,7 @@
         <v>0.208069</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="28">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="28">
       <c r="E28" s="0" t="s">
         <v>178</v>
       </c>
@@ -4709,7 +4625,7 @@
         <v>0.224594</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="29">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="29">
       <c r="E29" s="0" t="s">
         <v>185</v>
       </c>
@@ -4753,7 +4669,7 @@
         <v>0.194823</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="30">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="30">
       <c r="E30" s="0" t="s">
         <v>192</v>
       </c>
@@ -4797,7 +4713,7 @@
         <v>0.209605</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="31">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="31">
       <c r="E31" s="0" t="s">
         <v>199</v>
       </c>
@@ -4841,7 +4757,7 @@
         <v>0.190416</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="32">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="32">
       <c r="E32" s="0" t="s">
         <v>206</v>
       </c>
@@ -4885,7 +4801,7 @@
         <v>0.203897</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="33">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="33">
       <c r="E33" s="0" t="s">
         <v>213</v>
       </c>
@@ -4929,7 +4845,7 @@
         <v>0.155259</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="34">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="34">
       <c r="E34" s="0" t="s">
         <v>220</v>
       </c>
@@ -4973,7 +4889,7 @@
         <v>0.166986</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="35">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="35">
       <c r="E35" s="0" t="s">
         <v>227</v>
       </c>
@@ -5017,7 +4933,7 @@
         <v>0.18192</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="36">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="36">
       <c r="E36" s="0" t="s">
         <v>234</v>
       </c>
@@ -5061,7 +4977,7 @@
         <v>0.196236</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="37">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="37">
       <c r="E37" s="0" t="s">
         <v>241</v>
       </c>
@@ -5105,7 +5021,7 @@
         <v>0.190314</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="38">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="38">
       <c r="E38" s="0" t="s">
         <v>248</v>
       </c>
@@ -5149,7 +5065,7 @@
         <v>0.207021</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="39">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="39">
       <c r="F39" s="0" t="n">
         <f aca="false">AVERAGE(F3:F38)</f>
         <v>0.0516210944444444</v>
@@ -5179,7 +5095,7 @@
         <v>0.196459944444444</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="41">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="41">
       <c r="B41" s="0" t="n">
         <v>0</v>
       </c>
@@ -5205,7 +5121,7 @@
         <v>0.1964599444</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="42">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="42">
       <c r="B42" s="0" t="n">
         <v>211</v>
       </c>
@@ -5231,12 +5147,12 @@
         <v>1026</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="52">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="52">
       <c r="C52" s="0" t="s">
         <v>255</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="53">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="53">
       <c r="C53" s="0" t="s">
         <v>256</v>
       </c>
@@ -5265,7 +5181,7 @@
         <v>200</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="54">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="54">
       <c r="C54" s="0" t="s">
         <v>257</v>
       </c>
@@ -5294,7 +5210,7 @@
         <v>84</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="55">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="55">
       <c r="C55" s="0" t="s">
         <v>258</v>
       </c>
@@ -5331,7 +5247,7 @@
         <v>419</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="56">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="56">
       <c r="C56" s="0" t="s">
         <v>259</v>
       </c>
@@ -5360,7 +5276,7 @@
         <v>58</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="57">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="57">
       <c r="E57" s="0" t="n">
         <v>920</v>
       </c>
@@ -5386,7 +5302,7 @@
         <v>503</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="59">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="59">
       <c r="D59" s="1" t="n">
         <v>0</v>
       </c>
@@ -5412,7 +5328,7 @@
         <v>0.1964599444</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="60">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="60">
       <c r="C60" s="0" t="s">
         <v>257</v>
       </c>
@@ -5441,7 +5357,7 @@
         <v>106</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="61">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="61">
       <c r="C61" s="0" t="s">
         <v>258</v>
       </c>
@@ -5470,7 +5386,7 @@
         <v>850</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="62">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="62">
       <c r="C62" s="0" t="s">
         <v>259</v>
       </c>
@@ -5499,7 +5415,7 @@
         <v>140</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="63">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="63">
       <c r="D63" s="0" t="n">
         <v>0</v>
       </c>
@@ -5516,7 +5432,7 @@
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="64">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="64">
       <c r="D64" s="1" t="n">
         <v>0</v>
       </c>
@@ -5542,7 +5458,7 @@
         <v>0.1964599444</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="65">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="65">
       <c r="C65" s="0" t="s">
         <v>257</v>
       </c>
@@ -5571,7 +5487,7 @@
         <v>106</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="66">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="66">
       <c r="C66" s="0" t="s">
         <v>258</v>
       </c>
@@ -5600,7 +5516,7 @@
         <v>850</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="67">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="67">
       <c r="C67" s="0" t="s">
         <v>259</v>
       </c>
@@ -5629,7 +5545,7 @@
         <v>140</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="69">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="69">
       <c r="C69" s="2" t="s">
         <v>260</v>
       </c>
@@ -5650,7 +5566,7 @@
         <v>0.00495850330566887</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="70">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="70">
       <c r="C70" s="2" t="s">
         <v>262</v>
       </c>
@@ -5668,7 +5584,7 @@
         <v>0.00668167112111408</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="71">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="71">
       <c r="C71" s="2" t="s">
         <v>263</v>
       </c>
@@ -5689,7 +5605,7 @@
         <v>0.0111478407652272</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="72">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="72">
       <c r="C72" s="2" t="s">
         <v>264</v>
       </c>
@@ -5710,7 +5626,7 @@
         <v>0.0253200168800113</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="73">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="73">
       <c r="C73" s="2" t="s">
         <v>265</v>
       </c>
@@ -5731,7 +5647,7 @@
         <v>0.0512378674919117</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="74">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="74">
       <c r="C74" s="2" t="s">
         <v>266</v>
       </c>
@@ -5752,7 +5668,7 @@
         <v>0.103284568856379</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="75">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="75">
       <c r="C75" s="2" t="s">
         <v>267</v>
       </c>
@@ -5773,7 +5689,7 @@
         <v>0.201821634547756</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="76">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="76">
       <c r="C76" s="0" t="s">
         <v>268</v>
       </c>
@@ -5802,7 +5718,7 @@
         <v>128</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="77">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="77">
       <c r="D77" s="1" t="n">
         <v>0.00495850330566887</v>
       </c>
@@ -5828,12 +5744,12 @@
         <v>0.201821634547756</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="78">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="78">
       <c r="C78" s="0" t="s">
         <v>257</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="79">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="79">
       <c r="C79" s="0" t="s">
         <v>258</v>
       </c>
@@ -5856,7 +5772,7 @@
         <v>422</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="80">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="80">
       <c r="C80" s="0" t="s">
         <v>259</v>
       </c>
@@ -5885,7 +5801,7 @@
         <v>60</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="82">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="82">
       <c r="C82" s="0" t="s">
         <v>268</v>
       </c>
@@ -5923,7 +5839,7 @@
         <v>128</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="83">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="83">
       <c r="D83" s="1" t="n">
         <v>0.00495850330566887</v>
       </c>
@@ -5958,7 +5874,7 @@
         <v>0.201821634547756</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="84">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="84">
       <c r="C84" s="0" t="s">
         <v>257</v>
       </c>
@@ -5996,7 +5912,7 @@
         <v>78</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="85">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="85">
       <c r="C85" s="0" t="s">
         <v>258</v>
       </c>
@@ -6045,7 +5961,7 @@
         <v>344</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="86">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="86">
       <c r="C86" s="0" t="s">
         <v>259</v>
       </c>
@@ -6083,7 +5999,7 @@
         <v>60</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="88">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="88">
       <c r="D88" s="0" t="n">
         <v>392</v>
       </c>
@@ -6118,12 +6034,12 @@
         <v>422</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="91">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="91">
       <c r="A91" s="0" t="s">
         <v>269</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="92">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="92">
       <c r="B92" s="0" t="n">
         <v>0</v>
       </c>
@@ -6146,7 +6062,7 @@
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="93">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="93">
       <c r="B93" s="1" t="n">
         <v>0</v>
       </c>
@@ -6169,119 +6085,121 @@
         <v>0.073</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="94">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="94">
       <c r="A94" s="0" t="s">
         <v>257</v>
       </c>
       <c r="B94" s="0" t="n">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C94" s="0" t="n">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D94" s="0" t="n">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="E94" s="0" t="n">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="F94" s="0" t="n">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="G94" s="0" t="n">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="H94" s="0" t="n">
-        <v>84</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="95">
+        <v>70</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="95">
       <c r="A95" s="0" t="s">
         <v>258</v>
       </c>
       <c r="B95" s="0" t="n">
         <f aca="false">B97-B94</f>
-        <v>240</v>
+        <v>91</v>
       </c>
       <c r="C95" s="0" t="n">
         <f aca="false">C97-C94</f>
-        <v>282</v>
+        <v>92</v>
       </c>
       <c r="D95" s="0" t="n">
         <f aca="false">D97-D94</f>
-        <v>318</v>
+        <v>92</v>
       </c>
       <c r="E95" s="0" t="n">
-        <v>342</v>
+        <f aca="false">E97-E94</f>
+        <v>97</v>
       </c>
       <c r="F95" s="0" t="n">
         <f aca="false">F97-F94</f>
-        <v>362</v>
+        <v>100</v>
       </c>
       <c r="G95" s="0" t="n">
         <f aca="false">G97-G94</f>
-        <v>368</v>
+        <v>101</v>
       </c>
       <c r="H95" s="0" t="n">
         <f aca="false">H97-H94</f>
-        <v>379</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="96">
+        <v>102</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="96">
       <c r="A96" s="0" t="s">
         <v>259</v>
       </c>
       <c r="B96" s="0" t="n">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="C96" s="0" t="n">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="D96" s="0" t="n">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="E96" s="0" t="n">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="F96" s="0" t="n">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="G96" s="0" t="n">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="H96" s="0" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="97">
+        <v>45</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="97">
       <c r="B97" s="0" t="n">
-        <v>320</v>
+        <v>157</v>
       </c>
       <c r="C97" s="0" t="n">
-        <v>362</v>
+        <v>159</v>
       </c>
       <c r="D97" s="0" t="n">
-        <v>398</v>
+        <v>160</v>
       </c>
       <c r="E97" s="0" t="n">
-        <v>437</v>
+        <v>165</v>
       </c>
       <c r="F97" s="0" t="n">
-        <v>444</v>
+        <v>168</v>
       </c>
       <c r="G97" s="0" t="n">
-        <v>450</v>
+        <v>170</v>
       </c>
       <c r="H97" s="0" t="n">
-        <v>463</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="99">
+        <v>172</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="98"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="99">
       <c r="A99" s="0" t="s">
         <v>270</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="100">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="100">
       <c r="B100" s="0" t="n">
         <v>0</v>
       </c>
@@ -6304,7 +6222,7 @@
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="101">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="101">
       <c r="B101" s="1" t="n">
         <v>0</v>
       </c>
@@ -6327,7 +6245,7 @@
         <v>0.073</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="102">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="102">
       <c r="A102" s="0" t="s">
         <v>257</v>
       </c>
@@ -6353,40 +6271,40 @@
         <v>84</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="103">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="103">
       <c r="A103" s="0" t="s">
         <v>258</v>
       </c>
       <c r="B103" s="0" t="n">
         <f aca="false">B95*B106</f>
-        <v>258.96</v>
+        <v>98.189</v>
       </c>
       <c r="C103" s="0" t="n">
         <f aca="false">C95*C106</f>
-        <v>300.33</v>
+        <v>97.98</v>
       </c>
       <c r="D103" s="0" t="n">
         <f aca="false">D95*D106</f>
-        <v>334.218</v>
+        <v>96.692</v>
       </c>
       <c r="E103" s="0" t="n">
         <f aca="false">E95*E106</f>
-        <v>354.996</v>
+        <v>100.686</v>
       </c>
       <c r="F103" s="0" t="n">
         <f aca="false">F95*F106</f>
-        <v>371.05</v>
+        <v>102.5</v>
       </c>
       <c r="G103" s="0" t="n">
         <f aca="false">G95*G106</f>
-        <v>372.5264</v>
+        <v>102.2423</v>
       </c>
       <c r="H103" s="0" t="n">
         <f aca="false">H95*H106</f>
-        <v>379</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="104">
+        <v>102</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="104">
       <c r="A104" s="0" t="s">
         <v>259</v>
       </c>
@@ -6412,7 +6330,7 @@
         <v>60</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="106">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="106">
       <c r="A106" s="0" t="s">
         <v>271</v>
       </c>
@@ -6462,10 +6380,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="2">
       <c r="A2" s="0" t="n">
         <v>2</v>
       </c>
@@ -6509,7 +6427,7 @@
         <v>278</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="3">
       <c r="A3" s="0" t="n">
         <v>1440</v>
       </c>
@@ -6553,7 +6471,7 @@
         <v>34196</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="4">
       <c r="A4" s="0" t="n">
         <v>1366</v>
       </c>
@@ -6597,7 +6515,7 @@
         <v>30483</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="5">
       <c r="A5" s="0" t="n">
         <v>7734</v>
       </c>
@@ -6641,7 +6559,7 @@
         <v>190590</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="6">
       <c r="A6" s="0" t="n">
         <v>8084</v>
       </c>
@@ -6685,7 +6603,7 @@
         <v>185064</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="7">
       <c r="A7" s="0" t="n">
         <v>2186</v>
       </c>
@@ -6729,7 +6647,7 @@
         <v>49466</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="8">
       <c r="A8" s="0" t="n">
         <v>22320</v>
       </c>
@@ -6773,7 +6691,7 @@
         <v>454160</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="9">
       <c r="A9" s="0" t="n">
         <v>24812</v>
       </c>
@@ -6817,7 +6735,7 @@
         <v>515463</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="10">
       <c r="A10" s="0" t="n">
         <v>22488</v>
       </c>
@@ -6861,7 +6779,7 @@
         <v>435023</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="11">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="11">
       <c r="A11" s="0" t="n">
         <v>24822</v>
       </c>
@@ -6905,7 +6823,7 @@
         <v>636063</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="12">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="12">
       <c r="A12" s="0" t="n">
         <v>28322</v>
       </c>
@@ -6949,7 +6867,7 @@
         <v>668182</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="13">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="13">
       <c r="A13" s="0" t="n">
         <v>10220</v>
       </c>
@@ -6993,7 +6911,7 @@
         <v>220796</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="14">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="14">
       <c r="A14" s="0" t="n">
         <v>8990</v>
       </c>
@@ -7037,7 +6955,7 @@
         <v>178228</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="15">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="15">
       <c r="A15" s="0" t="n">
         <v>14152</v>
       </c>
@@ -7081,7 +6999,7 @@
         <v>350880</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="16">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="16">
       <c r="A16" s="0" t="n">
         <v>14540</v>
       </c>
@@ -7125,7 +7043,7 @@
         <v>337076</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="17">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="17">
       <c r="A17" s="0" t="n">
         <v>5532</v>
       </c>
@@ -7169,7 +7087,7 @@
         <v>127425</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="18">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="18">
       <c r="A18" s="0" t="n">
         <v>5022</v>
       </c>
@@ -7213,7 +7131,7 @@
         <v>106135</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="19">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="19">
       <c r="A19" s="0" t="n">
         <v>16792</v>
       </c>
@@ -7257,7 +7175,7 @@
         <v>452916</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="20">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="20">
       <c r="A20" s="0" t="n">
         <v>17178</v>
       </c>
@@ -7301,7 +7219,7 @@
         <v>419155</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="21">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="21">
       <c r="A21" s="0" t="n">
         <v>22890</v>
       </c>
@@ -7345,7 +7263,7 @@
         <v>602003</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="22">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="22">
       <c r="A22" s="0" t="n">
         <v>21832</v>
       </c>
@@ -7389,7 +7307,7 @@
         <v>523855</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="23">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="23">
       <c r="A23" s="0" t="n">
         <v>12568</v>
       </c>
@@ -7433,7 +7351,7 @@
         <v>273046</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="24">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="24">
       <c r="A24" s="0" t="n">
         <v>11364</v>
       </c>
@@ -7477,7 +7395,7 @@
         <v>232918</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="25">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="25">
       <c r="A25" s="0" t="n">
         <v>38862</v>
       </c>
@@ -7521,7 +7439,7 @@
         <v>948797</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="26">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="26">
       <c r="A26" s="0" t="n">
         <v>36690</v>
       </c>
@@ -7565,7 +7483,7 @@
         <v>836351</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="27">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="27">
       <c r="A27" s="0" t="n">
         <v>26210</v>
       </c>
@@ -7609,7 +7527,7 @@
         <v>566856</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="28">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="28">
       <c r="A28" s="0" t="n">
         <v>27192</v>
       </c>
@@ -7653,7 +7571,7 @@
         <v>544823</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="29">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="29">
       <c r="A29" s="0" t="n">
         <v>27650</v>
       </c>
@@ -7697,7 +7615,7 @@
         <v>638658</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="30">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="30">
       <c r="A30" s="0" t="n">
         <v>26628</v>
       </c>
@@ -7741,7 +7659,7 @@
         <v>571675</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="31">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="31">
       <c r="A31" s="0" t="n">
         <v>36316</v>
       </c>
@@ -7785,7 +7703,7 @@
         <v>858237</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="32">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="32">
       <c r="A32" s="0" t="n">
         <v>31870</v>
       </c>
@@ -7829,7 +7747,7 @@
         <v>703370</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="33">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="33">
       <c r="A33" s="0" t="n">
         <v>17040</v>
       </c>
@@ -7873,7 +7791,7 @@
         <v>493884</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="34">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="34">
       <c r="A34" s="0" t="n">
         <v>17210</v>
       </c>
@@ -7917,7 +7835,7 @@
         <v>463781</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="35">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="35">
       <c r="A35" s="0" t="n">
         <v>37804</v>
       </c>
@@ -7961,7 +7879,7 @@
         <v>935127</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="36">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="36">
       <c r="A36" s="0" t="n">
         <v>39412</v>
       </c>
@@ -8005,7 +7923,7 @@
         <v>903779</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="37">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="37">
       <c r="A37" s="0" t="n">
         <v>103412</v>
       </c>
@@ -8049,7 +7967,7 @@
         <v>2445196</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="38">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="38">
       <c r="A38" s="0" t="n">
         <v>94130</v>
       </c>
@@ -8093,7 +8011,7 @@
         <v>2046100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="39">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="39">
       <c r="A39" s="3" t="n">
         <f aca="false">SUM(A3:A38)</f>
         <v>865080</v>
@@ -8151,7 +8069,7 @@
         <v>19979757</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="40">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="40">
       <c r="B40" s="0" t="n">
         <f aca="false">A39/B39</f>
         <v>0.0510312160050713</v>
@@ -8181,7 +8099,7 @@
         <v>0.194840207516037</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="42">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.1" outlineLevel="0" r="42">
       <c r="B42" s="0" t="n">
         <v>75</v>
       </c>
@@ -8227,7 +8145,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>